<commit_message>
modified simulation of data
</commit_message>
<xml_diff>
--- a/Data Simulation/simulated_data.xlsx
+++ b/Data Simulation/simulated_data.xlsx
@@ -687,44 +687,44 @@
         <v>21889.03123230718</v>
       </c>
       <c r="Q2" t="n">
-        <v>6625.268669500442</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>4417.109212488454</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>-17571.49950903812</v>
+        <v>15554.84383846409</v>
       </c>
       <c r="T2" t="n">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="U2" t="n">
-        <v>50467.83524282663</v>
+        <v>130672.5018699766</v>
       </c>
       <c r="V2" t="n">
-        <v>476737.8513074535</v>
+        <v>776666.1140470143</v>
       </c>
       <c r="W2" t="n">
-        <v>13193.36824138826</v>
+        <v>18882.39501835127</v>
       </c>
       <c r="X2" t="n">
-        <v>387126.4267187261</v>
+        <v>438926.6492088101</v>
       </c>
       <c r="Y2" t="n">
-        <v>184200.7096796019</v>
+        <v>696517.4566331406</v>
       </c>
       <c r="Z2" t="n">
-        <v>18092.95488419027</v>
+        <v>9571.926512375001</v>
       </c>
       <c r="AA2" t="n">
-        <v>217980.8378524647</v>
+        <v>456991.2390601542</v>
       </c>
       <c r="AB2" t="n">
-        <v>270297.0216009922</v>
+        <v>267533.8774694387</v>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>Balanced</t>
+          <t>High Growth</t>
         </is>
       </c>
       <c r="AD2" t="b">
@@ -743,16 +743,16 @@
         <v>0</v>
       </c>
       <c r="AI2" t="n">
-        <v>730122.0295167697</v>
+        <v>174908.8743095075</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.05802916032387562</v>
+        <v>0.09259616511851354</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.5365792111087222</v>
+        <v>0.009240073486540767</v>
       </c>
       <c r="AL2" t="n">
-        <v>294.1585567768029</v>
+        <v>227.5844075966687</v>
       </c>
     </row>
     <row r="3">
@@ -803,40 +803,40 @@
         <v>12693.2289346606</v>
       </c>
       <c r="Q3" t="n">
-        <v>135.7163561210983</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>9795.867288127285</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>60855.27354609149</v>
+        <v>61533.85532669698</v>
       </c>
       <c r="T3" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="U3" t="n">
-        <v>51112.11837869749</v>
+        <v>52799.45170986404</v>
       </c>
       <c r="V3" t="n">
-        <v>979642.3819996811</v>
+        <v>946917.3434636819</v>
       </c>
       <c r="W3" t="n">
-        <v>10664.12507833297</v>
+        <v>12165.05731708026</v>
       </c>
       <c r="X3" t="n">
-        <v>445303.4856242189</v>
+        <v>387879.9105327942</v>
       </c>
       <c r="Y3" t="n">
-        <v>142396.9307100152</v>
+        <v>131030.7875657655</v>
       </c>
       <c r="Z3" t="n">
-        <v>751.1876765628056</v>
+        <v>13541.63148054171</v>
       </c>
       <c r="AA3" t="n">
-        <v>239033.9164057748</v>
+        <v>340603.0693258547</v>
       </c>
       <c r="AB3" t="n">
-        <v>202543.3025509002</v>
+        <v>404932.7423894164</v>
       </c>
       <c r="AC3" t="inlineStr">
         <is>
@@ -859,16 +859,16 @@
         <v>0</v>
       </c>
       <c r="AI3" t="n">
-        <v>311944.9954796018</v>
+        <v>704474.2583934939</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.4344166255581208</v>
+        <v>0.2174504927055718</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.8966712930403421</v>
+        <v>0.8330380975093908</v>
       </c>
       <c r="AL3" t="n">
-        <v>415.5242276180952</v>
+        <v>439.4348708887354</v>
       </c>
     </row>
     <row r="4">
@@ -929,40 +929,40 @@
         <v>17640.10333520559</v>
       </c>
       <c r="Q4" t="n">
-        <v>6228.460955466695</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>3594.444639693215</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>5657.178546638579</v>
+        <v>36799.48332397205</v>
       </c>
       <c r="T4" t="n">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="U4" t="n">
-        <v>82358.70700937777</v>
+        <v>136419.9448274699</v>
       </c>
       <c r="V4" t="n">
-        <v>160391.8141317747</v>
+        <v>762499.2863315954</v>
       </c>
       <c r="W4" t="n">
-        <v>4610.660470126598</v>
+        <v>11933.10812590106</v>
       </c>
       <c r="X4" t="n">
-        <v>96288.5114120472</v>
+        <v>484020.3955052439</v>
       </c>
       <c r="Y4" t="n">
-        <v>984840.1292959391</v>
+        <v>103597.4160782679</v>
       </c>
       <c r="Z4" t="n">
-        <v>10166.30897157782</v>
+        <v>12140.90122232903</v>
       </c>
       <c r="AA4" t="n">
-        <v>72764.65177440675</v>
+        <v>196107.3374299094</v>
       </c>
       <c r="AB4" t="n">
-        <v>130770.6174130351</v>
+        <v>153248.8255119704</v>
       </c>
       <c r="AC4" t="inlineStr">
         <is>
@@ -985,16 +985,16 @@
         <v>0</v>
       </c>
       <c r="AI4" t="n">
-        <v>398221.0622160919</v>
+        <v>463150.1999901332</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0.3117958819941026</v>
+        <v>0.7492544170632397</v>
       </c>
       <c r="AK4" t="n">
-        <v>0.9903389473967044</v>
+        <v>0.984329434348122</v>
       </c>
       <c r="AL4" t="n">
-        <v>314.4909217955744</v>
+        <v>246.1341207525793</v>
       </c>
     </row>
     <row r="5">
@@ -1045,44 +1045,44 @@
         <v>18842.10468247587</v>
       </c>
       <c r="Q5" t="n">
-        <v>6736.596308357894</v>
+        <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>4808.935308361628</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>-2893.50495416882</v>
+        <v>30789.47658762065</v>
       </c>
       <c r="T5" t="n">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="U5" t="n">
-        <v>42998.64185946132</v>
+        <v>69651.49919650386</v>
       </c>
       <c r="V5" t="n">
-        <v>778672.5183807904</v>
+        <v>372433.6284770427</v>
       </c>
       <c r="W5" t="n">
-        <v>7897.385869004583</v>
+        <v>15672.88490603777</v>
       </c>
       <c r="X5" t="n">
-        <v>91568.25025740419</v>
+        <v>299409.0957879981</v>
       </c>
       <c r="Y5" t="n">
-        <v>297323.8812080345</v>
+        <v>513445.819141016</v>
       </c>
       <c r="Z5" t="n">
-        <v>3336.950260969993</v>
+        <v>14293.93872474714</v>
       </c>
       <c r="AA5" t="n">
-        <v>214473.2478185346</v>
+        <v>283870.0371462243</v>
       </c>
       <c r="AB5" t="n">
-        <v>126943.9694074092</v>
+        <v>446133.921401752</v>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>Balanced</t>
+          <t>High Growth</t>
         </is>
       </c>
       <c r="AD5" t="b">
@@ -1101,16 +1101,16 @@
         <v>0</v>
       </c>
       <c r="AI5" t="n">
-        <v>209843.7489751221</v>
+        <v>840428.5325354325</v>
       </c>
       <c r="AJ5" t="n">
-        <v>0.6963434888154595</v>
+        <v>0.7316937564646905</v>
       </c>
       <c r="AK5" t="n">
-        <v>0.2168969843984739</v>
+        <v>0.7034947841347021</v>
       </c>
       <c r="AL5" t="n">
-        <v>436.3253277236976</v>
+        <v>357.7805787295199</v>
       </c>
     </row>
     <row r="6">
@@ -1161,40 +1161,40 @@
         <v>12996.94239027111</v>
       </c>
       <c r="Q6" t="n">
-        <v>9719.450024996657</v>
+        <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>6886.611828057704</v>
+        <v>6183.518460005614</v>
       </c>
       <c r="S6" t="n">
-        <v>11418.03792366116</v>
+        <v>60015.28804864444</v>
       </c>
       <c r="T6" t="n">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="U6" t="n">
-        <v>52683.20081595123</v>
+        <v>57465.8150156651</v>
       </c>
       <c r="V6" t="n">
-        <v>441229.1320166025</v>
+        <v>515071.490046539</v>
       </c>
       <c r="W6" t="n">
-        <v>12376.17129182714</v>
+        <v>10000.52595458603</v>
       </c>
       <c r="X6" t="n">
-        <v>209320.9979377146</v>
+        <v>145575.7245006389</v>
       </c>
       <c r="Y6" t="n">
-        <v>560171.3953069907</v>
+        <v>886954.3340915912</v>
       </c>
       <c r="Z6" t="n">
-        <v>15581.02039218071</v>
+        <v>9389.943661823419</v>
       </c>
       <c r="AA6" t="n">
-        <v>57482.58818024027</v>
+        <v>50024.91058925386</v>
       </c>
       <c r="AB6" t="n">
-        <v>258552.9398230173</v>
+        <v>191161.5766286134</v>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
@@ -1217,16 +1217,16 @@
         <v>0</v>
       </c>
       <c r="AI6" t="n">
-        <v>186193.0058803362</v>
+        <v>204865.7621804457</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0.3777518392924809</v>
+        <v>0.04561463715088643</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.6630782031001008</v>
+        <v>0.1816312004920487</v>
       </c>
       <c r="AL6" t="n">
-        <v>136.7710174078179</v>
+        <v>243.0797801555988</v>
       </c>
     </row>
     <row r="7">
@@ -1277,44 +1277,44 @@
         <v>20841.64827164227</v>
       </c>
       <c r="Q7" t="n">
-        <v>8781.93471347177</v>
+        <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>8804.758892525955</v>
+        <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>-23117.91492557018</v>
+        <v>20791.75864178867</v>
       </c>
       <c r="T7" t="n">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="U7" t="n">
-        <v>41882.94826270087</v>
+        <v>58401.50739581222</v>
       </c>
       <c r="V7" t="n">
-        <v>691667.1271402242</v>
+        <v>372035.8609407893</v>
       </c>
       <c r="W7" t="n">
-        <v>9497.35030817884</v>
+        <v>1007.401135150876</v>
       </c>
       <c r="X7" t="n">
-        <v>298317.3166099665</v>
+        <v>150099.4509740684</v>
       </c>
       <c r="Y7" t="n">
-        <v>475529.8632771934</v>
+        <v>977584.1672633904</v>
       </c>
       <c r="Z7" t="n">
-        <v>17298.66591204985</v>
+        <v>9120.292464357344</v>
       </c>
       <c r="AA7" t="n">
-        <v>153834.0509330581</v>
+        <v>190337.0993069851</v>
       </c>
       <c r="AB7" t="n">
-        <v>443557.8309402484</v>
+        <v>480852.8850465292</v>
       </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>High Growth</t>
+          <t>Balanced</t>
         </is>
       </c>
       <c r="AD7" t="b">
@@ -1333,16 +1333,16 @@
         <v>0</v>
       </c>
       <c r="AI7" t="n">
-        <v>944372.3899839335</v>
+        <v>164958.8680867573</v>
       </c>
       <c r="AJ7" t="n">
-        <v>0.1796036775596348</v>
+        <v>0.2091570294808411</v>
       </c>
       <c r="AK7" t="n">
-        <v>0.2633223767371506</v>
+        <v>0.5123934632959037</v>
       </c>
       <c r="AL7" t="n">
-        <v>399.0234169562818</v>
+        <v>354.2740750100015</v>
       </c>
     </row>
     <row r="8">
@@ -1393,44 +1393,44 @@
         <v>12249.83612138016</v>
       </c>
       <c r="Q8" t="n">
-        <v>5096.243767199001</v>
+        <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>9182.354663621447</v>
+        <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>38269.60055710421</v>
+        <v>63750.81939309922</v>
       </c>
       <c r="T8" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="U8" t="n">
-        <v>56881.15162527231</v>
+        <v>51011.76230108475</v>
       </c>
       <c r="V8" t="n">
-        <v>287306.4618722292</v>
+        <v>220515.7478719629</v>
       </c>
       <c r="W8" t="n">
-        <v>9402.643785115304</v>
+        <v>13981.96149437022</v>
       </c>
       <c r="X8" t="n">
-        <v>65131.29207447441</v>
+        <v>148437.2181815473</v>
       </c>
       <c r="Y8" t="n">
-        <v>144590.6346552705</v>
+        <v>636775.0202910862</v>
       </c>
       <c r="Z8" t="n">
-        <v>8227.93447510909</v>
+        <v>18128.36174120342</v>
       </c>
       <c r="AA8" t="n">
-        <v>394210.2645485858</v>
+        <v>241453.1920784792</v>
       </c>
       <c r="AB8" t="n">
-        <v>474853.8879129036</v>
+        <v>262288.2069017605</v>
       </c>
       <c r="AC8" t="inlineStr">
         <is>
-          <t>Balanced</t>
+          <t>High Growth</t>
         </is>
       </c>
       <c r="AD8" t="b">
@@ -1449,16 +1449,16 @@
         <v>0</v>
       </c>
       <c r="AI8" t="n">
-        <v>739550.7950492876</v>
+        <v>124833.057490086</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0.02467872839133123</v>
+        <v>0.2869150433006046</v>
       </c>
       <c r="AK8" t="n">
-        <v>0.02065099946572868</v>
+        <v>0.5804471371881301</v>
       </c>
       <c r="AL8" t="n">
-        <v>92.8179721529761</v>
+        <v>249.070112753735</v>
       </c>
     </row>
     <row r="9">
@@ -1509,40 +1509,40 @@
         <v>13972.01082823012</v>
       </c>
       <c r="Q9" t="n">
-        <v>557.1469370160631</v>
+        <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>2168.221376275429</v>
+        <v>677.8165367962301</v>
       </c>
       <c r="S9" t="n">
-        <v>52354.21117376908</v>
+        <v>55139.94585884939</v>
       </c>
       <c r="T9" t="n">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="U9" t="n">
-        <v>49167.63228693939</v>
+        <v>57309.9221252682</v>
       </c>
       <c r="V9" t="n">
-        <v>347557.4153486534</v>
+        <v>212437.2687489749</v>
       </c>
       <c r="W9" t="n">
-        <v>14321.49062457286</v>
+        <v>19847.92797777265</v>
       </c>
       <c r="X9" t="n">
-        <v>486032.7943671232</v>
+        <v>306308.0905586321</v>
       </c>
       <c r="Y9" t="n">
-        <v>384696.0781405064</v>
+        <v>565373.8362598775</v>
       </c>
       <c r="Z9" t="n">
-        <v>2799.451709864034</v>
+        <v>2744.408401943892</v>
       </c>
       <c r="AA9" t="n">
-        <v>474855.5837459546</v>
+        <v>448401.9468243135</v>
       </c>
       <c r="AB9" t="n">
-        <v>323713.7896343058</v>
+        <v>370212.7176773662</v>
       </c>
       <c r="AC9" t="inlineStr">
         <is>
@@ -1565,16 +1565,16 @@
         <v>0</v>
       </c>
       <c r="AI9" t="n">
-        <v>490458.8086175671</v>
+        <v>722080.6624027486</v>
       </c>
       <c r="AJ9" t="n">
-        <v>0.06724963146324858</v>
+        <v>0.6772633053384269</v>
       </c>
       <c r="AK9" t="n">
-        <v>0.7583786538361414</v>
+        <v>0.7875421559550259</v>
       </c>
       <c r="AL9" t="n">
-        <v>476.3958284859723</v>
+        <v>422.2750397359712</v>
       </c>
     </row>
     <row r="10">
@@ -1625,40 +1625,40 @@
         <v>15302.58805299926</v>
       </c>
       <c r="Q10" t="n">
-        <v>4511.592145209281</v>
+        <v>9222.339545700042</v>
       </c>
       <c r="R10" t="n">
-        <v>5651.888666048753</v>
+        <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>25929.09900895727</v>
+        <v>2375.362006503465</v>
       </c>
       <c r="T10" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="U10" t="n">
-        <v>56746.63311677031</v>
+        <v>50332.55947467734</v>
       </c>
       <c r="V10" t="n">
-        <v>967145.4094939306</v>
+        <v>490278.4285152588</v>
       </c>
       <c r="W10" t="n">
-        <v>5759.82008726561</v>
+        <v>5345.250757629565</v>
       </c>
       <c r="X10" t="n">
-        <v>194448.7586180739</v>
+        <v>253449.0657650416</v>
       </c>
       <c r="Y10" t="n">
-        <v>495786.71529073</v>
+        <v>861882.9012951787</v>
       </c>
       <c r="Z10" t="n">
-        <v>664.4477053235454</v>
+        <v>4584.386461731588</v>
       </c>
       <c r="AA10" t="n">
-        <v>387499.6619465452</v>
+        <v>355945.7553830463</v>
       </c>
       <c r="AB10" t="n">
-        <v>318494.9328327739</v>
+        <v>119162.4372535084</v>
       </c>
       <c r="AC10" t="inlineStr">
         <is>
@@ -1681,16 +1681,16 @@
         <v>0</v>
       </c>
       <c r="AI10" t="n">
-        <v>227414.6279733232</v>
+        <v>30452.96494160032</v>
       </c>
       <c r="AJ10" t="n">
-        <v>0.6793927734985673</v>
+        <v>0.06303828966937675</v>
       </c>
       <c r="AK10" t="n">
-        <v>0.3200171508224678</v>
+        <v>0.6064754600685757</v>
       </c>
       <c r="AL10" t="n">
-        <v>343.7441381939076</v>
+        <v>97.1711114714916</v>
       </c>
     </row>
     <row r="11">
@@ -1751,44 +1751,44 @@
         <v>22323.7959283555</v>
       </c>
       <c r="Q11" t="n">
-        <v>199.8766540875874</v>
+        <v>0</v>
       </c>
       <c r="R11" t="n">
-        <v>8651.025613053849</v>
+        <v>0</v>
       </c>
       <c r="S11" t="n">
-        <v>12381.63708778457</v>
+        <v>13381.0203582225</v>
       </c>
       <c r="T11" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="U11" t="n">
-        <v>57322.08813645561</v>
+        <v>138958.5234374146</v>
       </c>
       <c r="V11" t="n">
-        <v>609041.8308153119</v>
+        <v>880844.3097627467</v>
       </c>
       <c r="W11" t="n">
-        <v>7669.244500698957</v>
+        <v>13581.81231254828</v>
       </c>
       <c r="X11" t="n">
-        <v>149568.2083327023</v>
+        <v>486606.5073932452</v>
       </c>
       <c r="Y11" t="n">
-        <v>849083.1232963195</v>
+        <v>756642.8180442983</v>
       </c>
       <c r="Z11" t="n">
-        <v>19651.49919650387</v>
+        <v>17631.70798421161</v>
       </c>
       <c r="AA11" t="n">
-        <v>202731.7187522834</v>
+        <v>255258.3974552879</v>
       </c>
       <c r="AB11" t="n">
-        <v>402639.9103858498</v>
+        <v>378698.9794550575</v>
       </c>
       <c r="AC11" t="inlineStr">
         <is>
-          <t>High Growth</t>
+          <t>Balanced</t>
         </is>
       </c>
       <c r="AD11" t="b">
@@ -1807,16 +1807,16 @@
         <v>0</v>
       </c>
       <c r="AI11" t="n">
-        <v>254356.4817703929</v>
+        <v>746994.2401995035</v>
       </c>
       <c r="AJ11" t="n">
-        <v>0.4536968445560453</v>
+        <v>0.5556492427701452</v>
       </c>
       <c r="AK11" t="n">
-        <v>0.383463894171898</v>
+        <v>0.2184028548119228</v>
       </c>
       <c r="AL11" t="n">
-        <v>107.7538385567792</v>
+        <v>386.6630048052849</v>
       </c>
     </row>
   </sheetData>

</xml_diff>